<commit_message>
small fix for Dry Clap 1
</commit_message>
<xml_diff>
--- a/presets.xlsx
+++ b/presets.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B59D1A54-C771-4F9D-895A-793E27B91707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5730E71-BCDD-4DE1-8807-FD559715CCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7065" yWindow="930" windowWidth="38700" windowHeight="17595" xr2:uid="{2896A2DA-B100-4C06-828A-2BC2331A2C75}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="presets" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="761">
   <si>
     <t xml:space="preserve">WGGL </t>
   </si>
@@ -2314,6 +2314,9 @@
   </si>
   <si>
     <t>The Rhythmica (dup)</t>
+  </si>
+  <si>
+    <t>Dry Clap 1 (dup)</t>
   </si>
 </sst>
 </file>
@@ -2677,7 +2680,7 @@
   <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4217,7 +4220,7 @@
         <v>405</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>760</v>
       </c>
       <c r="D40" t="s">
         <v>434</v>

</xml_diff>